<commit_message>
Ajout de mu-plugin, changement de page de connexion, début du javascript pour l'emploi du temps
</commit_message>
<xml_diff>
--- a/wp-content/plugins/TeleConnecteeAmu/Excel/vide.xlsx
+++ b/wp-content/plugins/TeleConnecteeAmu/Excel/vide.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ptut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\wpTv\wp-content\plugins\TeleConnecteeAmu\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB69EB2-ABA8-4589-A561-8E320DE37128}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Prénom</t>
   </si>
@@ -38,16 +39,10 @@
     <t>eMail</t>
   </si>
   <si>
-    <t>Alternant</t>
-  </si>
-  <si>
     <t>Groupe</t>
   </si>
   <si>
     <t>Demi-groupe</t>
-  </si>
-  <si>
-    <t>Langue</t>
   </si>
   <si>
     <t>Numéro Ent</t>
@@ -56,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,21 +373,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="7" max="8" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+    <col min="7" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +395,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -414,17 +409,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
     </row>
   </sheetData>

</xml_diff>